<commit_message>
Give credit where credit is due
</commit_message>
<xml_diff>
--- a/802.11ac-wave-2-model.xlsx
+++ b/802.11ac-wave-2-model.xlsx
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="325">
   <si>
     <t>1 SS</t>
   </si>
@@ -1247,6 +1247,9 @@
   </si>
   <si>
     <t>7.  View your results in the "OUT-wave2" tab, which shows throughput as a function of 11ac client capabilities.  Weights for legacy clients are maintained.</t>
+  </si>
+  <si>
+    <t>Should have noted that the wave 2 output tab was fixed in response to a bug report from Jonathan Hurtt.  Sorry, Jonathan…</t>
   </si>
 </sst>
 </file>
@@ -1365,9 +1368,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="394">
+  <cellStyleXfs count="396">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1810,6 +1815,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1819,10 +1825,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1831,9 +1837,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="394">
+  <cellStyles count="396">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2030,6 +2035,7 @@
     <cellStyle name="Followed Hyperlink" xfId="389" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="391" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="393" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="395" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2226,10 +2232,31 @@
     <cellStyle name="Hyperlink" xfId="388" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="390" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="392" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="394" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="30">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2332,26 +2359,6 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2668,11 +2675,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2127662328"/>
-        <c:axId val="2127666520"/>
+        <c:axId val="-2122693224"/>
+        <c:axId val="2127858920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2127662328"/>
+        <c:axId val="-2122693224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2700,7 +2707,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127666520"/>
+        <c:crossAx val="2127858920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2708,7 +2715,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127666520"/>
+        <c:axId val="2127858920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2718,7 +2725,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127662328"/>
+        <c:crossAx val="-2122693224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2952,11 +2959,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2114412088"/>
-        <c:axId val="-2114409112"/>
+        <c:axId val="-2122895368"/>
+        <c:axId val="-2122892392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2114412088"/>
+        <c:axId val="-2122895368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2965,7 +2972,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114409112"/>
+        <c:crossAx val="-2122892392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2973,7 +2980,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114409112"/>
+        <c:axId val="-2122892392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3002,7 +3009,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114412088"/>
+        <c:crossAx val="-2122895368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3485,11 +3492,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2114505736"/>
-        <c:axId val="-2114502760"/>
+        <c:axId val="2127709160"/>
+        <c:axId val="2127701576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2114505736"/>
+        <c:axId val="2127709160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3498,7 +3505,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114502760"/>
+        <c:crossAx val="2127701576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3506,7 +3513,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114502760"/>
+        <c:axId val="2127701576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3535,7 +3542,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114505736"/>
+        <c:crossAx val="2127709160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3885,11 +3892,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2135379800"/>
-        <c:axId val="2135382792"/>
+        <c:axId val="2127611720"/>
+        <c:axId val="2127610568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2135379800"/>
+        <c:axId val="2127611720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3898,7 +3905,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135382792"/>
+        <c:crossAx val="2127610568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3906,7 +3913,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2135382792"/>
+        <c:axId val="2127610568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3917,7 +3924,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135379800"/>
+        <c:crossAx val="2127611720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4080,7 +4087,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4770,11 +4776,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127569240"/>
-        <c:axId val="2127566856"/>
+        <c:axId val="2134953528"/>
+        <c:axId val="2134942024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127569240"/>
+        <c:axId val="2134953528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4796,13 +4802,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="2127566856"/>
+        <c:crossAx val="2134942024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4810,7 +4815,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127566856"/>
+        <c:axId val="2134942024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.8"/>
@@ -4834,21 +4839,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127569240"/>
+        <c:crossAx val="2134953528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4893,7 +4896,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5583,11 +5585,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2135216008"/>
-        <c:axId val="2135196776"/>
+        <c:axId val="-2123821336"/>
+        <c:axId val="-2123698472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2135216008"/>
+        <c:axId val="-2123821336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5609,13 +5611,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="2135196776"/>
+        <c:crossAx val="-2123698472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5623,7 +5624,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2135196776"/>
+        <c:axId val="-2123698472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.8"/>
@@ -5652,21 +5653,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135216008"/>
+        <c:crossAx val="-2123821336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5804,11 +5803,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2032079992"/>
-        <c:axId val="2032055592"/>
+        <c:axId val="2127797160"/>
+        <c:axId val="2127785576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2032079992"/>
+        <c:axId val="2127797160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5835,7 +5834,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2032055592"/>
+        <c:crossAx val="2127785576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5843,7 +5842,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2032055592"/>
+        <c:axId val="2127785576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5853,7 +5852,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2032079992"/>
+        <c:crossAx val="2127797160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5905,7 +5904,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5964,11 +5962,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2114533112"/>
-        <c:axId val="-2114529960"/>
+        <c:axId val="2127593208"/>
+        <c:axId val="2127587784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2114533112"/>
+        <c:axId val="2127593208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5977,7 +5975,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114529960"/>
+        <c:crossAx val="2127587784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5985,7 +5983,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114529960"/>
+        <c:axId val="2127587784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6008,14 +6006,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114533112"/>
+        <c:crossAx val="2127593208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6062,7 +6059,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6253,11 +6249,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2114583496"/>
-        <c:axId val="-2114602920"/>
+        <c:axId val="-2122999864"/>
+        <c:axId val="-2123009288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2114583496"/>
+        <c:axId val="-2122999864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6279,14 +6275,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114602920"/>
+        <c:crossAx val="-2123009288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6294,7 +6289,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114602920"/>
+        <c:axId val="-2123009288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6317,21 +6312,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114583496"/>
+        <c:crossAx val="-2122999864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6381,7 +6374,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6564,11 +6556,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2135186376"/>
-        <c:axId val="2135172360"/>
+        <c:axId val="-2123064776"/>
+        <c:axId val="-2123061800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2135186376"/>
+        <c:axId val="-2123064776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6577,7 +6569,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135172360"/>
+        <c:crossAx val="-2123061800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6585,7 +6577,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2135172360"/>
+        <c:axId val="-2123061800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6608,21 +6600,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135186376"/>
+        <c:crossAx val="-2123064776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6672,7 +6662,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6782,7 +6771,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6910,7 +6898,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7026,7 +7013,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7217,11 +7203,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2114659416"/>
-        <c:axId val="-2114656440"/>
+        <c:axId val="2127562120"/>
+        <c:axId val="2127567768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2114659416"/>
+        <c:axId val="2127562120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7230,7 +7216,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114656440"/>
+        <c:crossAx val="2127567768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7238,7 +7224,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114656440"/>
+        <c:axId val="2127567768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7261,21 +7247,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114659416"/>
+        <c:crossAx val="2127562120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7325,7 +7309,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7441,7 +7424,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7784,11 +7766,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2030511576"/>
-        <c:axId val="2066055416"/>
+        <c:axId val="-2123428104"/>
+        <c:axId val="-2123461224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2030511576"/>
+        <c:axId val="-2123428104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7811,19 +7793,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066055416"/>
+        <c:crossAx val="-2123461224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2066055416"/>
+        <c:axId val="-2123461224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7846,14 +7827,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2030511576"/>
+        <c:crossAx val="-2123428104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8221,8 +8201,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2074985864"/>
-        <c:axId val="2074743320"/>
+        <c:axId val="-2123476952"/>
+        <c:axId val="-2123473960"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -8558,11 +8538,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2074739000"/>
-        <c:axId val="2074744744"/>
+        <c:axId val="-2123486984"/>
+        <c:axId val="-2123483656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2074985864"/>
+        <c:axId val="-2123476952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8572,12 +8552,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074743320"/>
+        <c:crossAx val="-2123473960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2074743320"/>
+        <c:axId val="-2123473960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8588,12 +8568,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074985864"/>
+        <c:crossAx val="-2123476952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2074744744"/>
+        <c:axId val="-2123483656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8603,12 +8583,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074739000"/>
+        <c:crossAx val="-2123486984"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2074739000"/>
+        <c:axId val="-2123486984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8618,14 +8598,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074744744"/>
+        <c:crossAx val="-2123483656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8770,11 +8749,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="-2114261992"/>
-        <c:axId val="-2114213432"/>
+        <c:axId val="2127754552"/>
+        <c:axId val="2127744968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2114261992"/>
+        <c:axId val="2127754552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8801,7 +8780,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114213432"/>
+        <c:crossAx val="2127744968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8809,7 +8788,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114213432"/>
+        <c:axId val="2127744968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8819,7 +8798,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114261992"/>
+        <c:crossAx val="2127754552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9671,11 +9650,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2143342536"/>
-        <c:axId val="2143335608"/>
+        <c:axId val="-2122835592"/>
+        <c:axId val="-2122830072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2143342536"/>
+        <c:axId val="-2122835592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9703,7 +9682,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143335608"/>
+        <c:crossAx val="-2122830072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9711,7 +9690,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2143335608"/>
+        <c:axId val="-2122830072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9740,7 +9719,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143342536"/>
+        <c:crossAx val="-2122835592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13754,17 +13733,17 @@
       <c r="E85" s="8"/>
     </row>
     <row r="86" spans="1:13">
-      <c r="A86" s="35" t="s">
+      <c r="A86" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="B86" s="35"/>
-      <c r="C86" s="35"/>
+      <c r="B86" s="36"/>
+      <c r="C86" s="36"/>
       <c r="D86" s="8"/>
-      <c r="E86" s="37" t="s">
+      <c r="E86" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="F86" s="37"/>
-      <c r="G86" s="37"/>
+      <c r="F86" s="39"/>
+      <c r="G86" s="39"/>
     </row>
     <row r="87" spans="1:13">
       <c r="B87" s="8" t="s">
@@ -13896,12 +13875,12 @@
       <c r="G93" s="11"/>
     </row>
     <row r="94" spans="1:13">
-      <c r="A94" s="34" t="s">
+      <c r="A94" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="B94" s="34"/>
-      <c r="C94" s="34"/>
-      <c r="D94" s="34"/>
+      <c r="B94" s="35"/>
+      <c r="C94" s="35"/>
+      <c r="D94" s="35"/>
       <c r="E94" s="8"/>
       <c r="F94" s="8"/>
     </row>
@@ -15330,20 +15309,20 @@
       </c>
     </row>
     <row r="144" spans="1:13">
-      <c r="A144" s="39" t="s">
+      <c r="A144" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="B144" s="39"/>
-      <c r="C144" s="39"/>
-      <c r="D144" s="39"/>
-      <c r="E144" s="39"/>
-      <c r="F144" s="39"/>
-      <c r="G144" s="39"/>
-      <c r="H144" s="39"/>
-      <c r="I144" s="39"/>
-      <c r="J144" s="39"/>
-      <c r="K144" s="39"/>
-      <c r="L144" s="39"/>
+      <c r="B144" s="40"/>
+      <c r="C144" s="40"/>
+      <c r="D144" s="40"/>
+      <c r="E144" s="40"/>
+      <c r="F144" s="40"/>
+      <c r="G144" s="40"/>
+      <c r="H144" s="40"/>
+      <c r="I144" s="40"/>
+      <c r="J144" s="40"/>
+      <c r="K144" s="40"/>
+      <c r="L144" s="40"/>
     </row>
     <row r="145" spans="1:13">
       <c r="A145" s="9"/>
@@ -15925,20 +15904,20 @@
       </c>
     </row>
     <row r="159" spans="1:13">
-      <c r="A159" s="39" t="s">
+      <c r="A159" s="40" t="s">
         <v>164</v>
       </c>
-      <c r="B159" s="39"/>
-      <c r="C159" s="39"/>
-      <c r="D159" s="39"/>
-      <c r="E159" s="39"/>
-      <c r="F159" s="39"/>
-      <c r="G159" s="39"/>
-      <c r="H159" s="39"/>
-      <c r="I159" s="39"/>
-      <c r="J159" s="39"/>
-      <c r="K159" s="39"/>
-      <c r="L159" s="39"/>
+      <c r="B159" s="40"/>
+      <c r="C159" s="40"/>
+      <c r="D159" s="40"/>
+      <c r="E159" s="40"/>
+      <c r="F159" s="40"/>
+      <c r="G159" s="40"/>
+      <c r="H159" s="40"/>
+      <c r="I159" s="40"/>
+      <c r="J159" s="40"/>
+      <c r="K159" s="40"/>
+      <c r="L159" s="40"/>
     </row>
     <row r="160" spans="1:13">
       <c r="A160" s="9"/>
@@ -16523,14 +16502,14 @@
       <c r="K173" s="11"/>
     </row>
     <row r="174" spans="1:13">
-      <c r="A174" s="35" t="s">
+      <c r="A174" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="B174" s="35"/>
-      <c r="C174" s="35"/>
-      <c r="D174" s="35"/>
-      <c r="E174" s="35"/>
-      <c r="F174" s="35"/>
+      <c r="B174" s="36"/>
+      <c r="C174" s="36"/>
+      <c r="D174" s="36"/>
+      <c r="E174" s="36"/>
+      <c r="F174" s="36"/>
     </row>
     <row r="175" spans="1:13">
       <c r="B175" t="s">
@@ -16746,23 +16725,23 @@
       <c r="F187" s="13"/>
     </row>
     <row r="188" spans="1:13">
-      <c r="A188" s="35" t="s">
+      <c r="A188" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="B188" s="35"/>
-      <c r="C188" s="35"/>
-      <c r="D188" s="35"/>
-      <c r="E188" s="35"/>
+      <c r="B188" s="36"/>
+      <c r="C188" s="36"/>
+      <c r="D188" s="36"/>
+      <c r="E188" s="36"/>
       <c r="F188" s="21"/>
       <c r="G188" s="8"/>
-      <c r="H188" s="37" t="s">
+      <c r="H188" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="I188" s="37"/>
-      <c r="J188" s="37"/>
-      <c r="K188" s="37"/>
-      <c r="L188" s="37"/>
-      <c r="M188" s="37"/>
+      <c r="I188" s="39"/>
+      <c r="J188" s="39"/>
+      <c r="K188" s="39"/>
+      <c r="L188" s="39"/>
+      <c r="M188" s="39"/>
     </row>
     <row r="189" spans="1:13">
       <c r="B189" s="8" t="s">
@@ -16973,14 +16952,14 @@
       <c r="L194" s="1"/>
     </row>
     <row r="195" spans="1:14">
-      <c r="A195" s="34" t="s">
+      <c r="A195" s="35" t="s">
         <v>175</v>
       </c>
-      <c r="B195" s="34"/>
-      <c r="C195" s="34"/>
-      <c r="D195" s="34"/>
-      <c r="E195" s="34"/>
-      <c r="F195" s="34"/>
+      <c r="B195" s="35"/>
+      <c r="C195" s="35"/>
+      <c r="D195" s="35"/>
+      <c r="E195" s="35"/>
+      <c r="F195" s="35"/>
       <c r="H195" s="23"/>
       <c r="I195" s="23"/>
       <c r="J195" s="23"/>
@@ -17175,13 +17154,13 @@
       <c r="G202" s="11"/>
     </row>
     <row r="203" spans="1:14">
-      <c r="A203" s="34" t="s">
+      <c r="A203" s="35" t="s">
         <v>295</v>
       </c>
-      <c r="B203" s="34"/>
-      <c r="C203" s="34"/>
-      <c r="D203" s="34"/>
-      <c r="E203" s="34"/>
+      <c r="B203" s="35"/>
+      <c r="C203" s="35"/>
+      <c r="D203" s="35"/>
+      <c r="E203" s="35"/>
     </row>
     <row r="204" spans="1:14">
       <c r="B204" s="8" t="s">
@@ -17519,12 +17498,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A34:L34"/>
-    <mergeCell ref="A47:L47"/>
-    <mergeCell ref="A60:L60"/>
-    <mergeCell ref="A73:L73"/>
-    <mergeCell ref="A86:C86"/>
-    <mergeCell ref="E86:G86"/>
     <mergeCell ref="A188:E188"/>
     <mergeCell ref="H188:M188"/>
     <mergeCell ref="A195:F195"/>
@@ -17535,6 +17508,12 @@
     <mergeCell ref="A144:L144"/>
     <mergeCell ref="A159:L159"/>
     <mergeCell ref="A174:F174"/>
+    <mergeCell ref="A34:L34"/>
+    <mergeCell ref="A47:L47"/>
+    <mergeCell ref="A60:L60"/>
+    <mergeCell ref="A73:L73"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="E86:G86"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -17597,7 +17576,7 @@
       <c r="J6" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="41">
+      <c r="K6" s="34">
         <f>'IN-client'!K6</f>
         <v>5</v>
       </c>
@@ -17606,7 +17585,7 @@
       <c r="A7" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="41">
+      <c r="B7" s="34">
         <f>IF(C$9=1,0,'IN-client'!B7)</f>
         <v>10</v>
       </c>
@@ -17617,7 +17596,7 @@
       <c r="J7" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="41">
+      <c r="K7" s="34">
         <f>'IN-client'!K7</f>
         <v>7</v>
       </c>
@@ -17626,18 +17605,18 @@
       <c r="A8" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="41">
+      <c r="B8" s="34">
         <f>IF(C$9=1,0,'IN-client'!B8)</f>
         <v>30</v>
       </c>
       <c r="C8" s="30">
-        <f t="shared" ref="C8:C9" si="0">B8/SUM(B$7:B$9)</f>
+        <f t="shared" ref="C8" si="0">B8/SUM(B$7:B$9)</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="J8" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="41">
+      <c r="K8" s="34">
         <f>'IN-client'!K8</f>
         <v>10</v>
       </c>
@@ -17646,7 +17625,7 @@
       <c r="A9" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="41">
+      <c r="B9" s="34">
         <f>IF(C9=1,1,C9*SUM(B7:B8)/(1-C9))</f>
         <v>50</v>
       </c>
@@ -17688,7 +17667,7 @@
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="41">
+      <c r="B14" s="34">
         <f>IF(C$17=1,0,'IN-client'!B14)</f>
         <v>50</v>
       </c>
@@ -17699,7 +17678,7 @@
       <c r="F14" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="41">
+      <c r="G14" s="34">
         <f>'IN-client'!G14</f>
         <v>0.7</v>
       </c>
@@ -17708,18 +17687,18 @@
       <c r="A15" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="41">
+      <c r="B15" s="34">
         <f>IF(C$17=1,0,'IN-client'!B15)</f>
         <v>25</v>
       </c>
       <c r="C15" s="30">
-        <f t="shared" ref="C15:C17" si="1">B15/SUM(B$14:B$17)</f>
+        <f t="shared" ref="C15:C16" si="1">B15/SUM(B$14:B$17)</f>
         <v>0.25</v>
       </c>
       <c r="F15" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="41">
+      <c r="G15" s="34">
         <f>'IN-client'!G15</f>
         <v>0.3</v>
       </c>
@@ -17728,7 +17707,7 @@
       <c r="A16" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="41">
+      <c r="B16" s="34">
         <f>IF(C$17=1,0,'IN-client'!B16)</f>
         <v>25</v>
       </c>
@@ -17749,7 +17728,7 @@
       <c r="A17" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="41">
+      <c r="B17" s="34">
         <f>IF(C17=1,1,C17*SUM(B14:B16)/(1-C17))</f>
         <v>0</v>
       </c>
@@ -17791,7 +17770,7 @@
       <c r="A22" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="41">
+      <c r="B22" s="34">
         <f>IF(C$25=1,0,'IN-client'!B22)</f>
         <v>35</v>
       </c>
@@ -17802,7 +17781,7 @@
       <c r="F22" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="41">
+      <c r="G22" s="34">
         <f>'IN-client'!G22</f>
         <v>0</v>
       </c>
@@ -17811,18 +17790,18 @@
       <c r="A23" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="41">
+      <c r="B23" s="34">
         <f>IF(C$25=1,0,'IN-client'!B23)</f>
         <v>20</v>
       </c>
       <c r="C23" s="30">
-        <f t="shared" ref="C23:C25" si="2">B23/SUM(B$22:B$25)</f>
+        <f t="shared" ref="C23:C24" si="2">B23/SUM(B$22:B$25)</f>
         <v>0.26666666666666666</v>
       </c>
       <c r="F23" t="s">
         <v>36</v>
       </c>
-      <c r="G23" s="41">
+      <c r="G23" s="34">
         <f>'IN-client'!G23</f>
         <v>0</v>
       </c>
@@ -17831,7 +17810,7 @@
       <c r="A24" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="41">
+      <c r="B24" s="34">
         <f>IF(C$25=1,0,'IN-client'!B24)</f>
         <v>20</v>
       </c>
@@ -17842,7 +17821,7 @@
       <c r="F24" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="41">
+      <c r="G24" s="34">
         <f>'IN-client'!G24</f>
         <v>1</v>
       </c>
@@ -17851,7 +17830,7 @@
       <c r="A25" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="41">
+      <c r="B25" s="34">
         <f>IF(C25=1,1,C25*SUM(B22:B24)/(1-C25))</f>
         <v>0</v>
       </c>
@@ -17866,7 +17845,7 @@
       <c r="F25" t="s">
         <v>39</v>
       </c>
-      <c r="G25" s="41">
+      <c r="G25" s="34">
         <f>'IN-client'!G25</f>
         <v>0</v>
       </c>
@@ -17904,7 +17883,7 @@
       <c r="A30" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="41">
+      <c r="B30" s="34">
         <f>'IN-client'!B30</f>
         <v>3</v>
       </c>
@@ -17918,7 +17897,7 @@
       <c r="A33" t="s">
         <v>95</v>
       </c>
-      <c r="B33" s="41">
+      <c r="B33" s="34">
         <f>'IN-client'!B33</f>
         <v>0</v>
       </c>
@@ -17927,49 +17906,49 @@
       <c r="A34" t="s">
         <v>96</v>
       </c>
-      <c r="B34" s="41">
+      <c r="B34" s="34">
         <f>'IN-client'!B34</f>
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D9">
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="11" priority="9">
       <formula>D9="OK"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="10" priority="10">
       <formula>D9="ERROR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="9" priority="7">
       <formula>D17="OK"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>D17="ERROR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>D25="OK"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>D25="ERROR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>H26="OK"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>H26="ERROR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>H16="OK"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>H16="ERROR"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20550,17 +20529,17 @@
       <c r="E85" s="8"/>
     </row>
     <row r="86" spans="1:13">
-      <c r="A86" s="35" t="s">
+      <c r="A86" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="B86" s="35"/>
-      <c r="C86" s="35"/>
+      <c r="B86" s="36"/>
+      <c r="C86" s="36"/>
       <c r="D86" s="8"/>
-      <c r="E86" s="37" t="s">
+      <c r="E86" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="F86" s="37"/>
-      <c r="G86" s="37"/>
+      <c r="F86" s="39"/>
+      <c r="G86" s="39"/>
     </row>
     <row r="87" spans="1:13">
       <c r="B87" s="8" t="s">
@@ -20692,12 +20671,12 @@
       <c r="G93" s="11"/>
     </row>
     <row r="94" spans="1:13">
-      <c r="A94" s="34" t="s">
+      <c r="A94" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="B94" s="34"/>
-      <c r="C94" s="34"/>
-      <c r="D94" s="34"/>
+      <c r="B94" s="35"/>
+      <c r="C94" s="35"/>
+      <c r="D94" s="35"/>
       <c r="E94" s="8"/>
       <c r="F94" s="8"/>
     </row>
@@ -22126,20 +22105,20 @@
       </c>
     </row>
     <row r="144" spans="1:13">
-      <c r="A144" s="39" t="s">
+      <c r="A144" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="B144" s="39"/>
-      <c r="C144" s="39"/>
-      <c r="D144" s="39"/>
-      <c r="E144" s="39"/>
-      <c r="F144" s="39"/>
-      <c r="G144" s="39"/>
-      <c r="H144" s="39"/>
-      <c r="I144" s="39"/>
-      <c r="J144" s="39"/>
-      <c r="K144" s="39"/>
-      <c r="L144" s="39"/>
+      <c r="B144" s="40"/>
+      <c r="C144" s="40"/>
+      <c r="D144" s="40"/>
+      <c r="E144" s="40"/>
+      <c r="F144" s="40"/>
+      <c r="G144" s="40"/>
+      <c r="H144" s="40"/>
+      <c r="I144" s="40"/>
+      <c r="J144" s="40"/>
+      <c r="K144" s="40"/>
+      <c r="L144" s="40"/>
     </row>
     <row r="145" spans="1:13">
       <c r="A145" s="9"/>
@@ -22721,20 +22700,20 @@
       </c>
     </row>
     <row r="159" spans="1:13">
-      <c r="A159" s="39" t="s">
+      <c r="A159" s="40" t="s">
         <v>164</v>
       </c>
-      <c r="B159" s="39"/>
-      <c r="C159" s="39"/>
-      <c r="D159" s="39"/>
-      <c r="E159" s="39"/>
-      <c r="F159" s="39"/>
-      <c r="G159" s="39"/>
-      <c r="H159" s="39"/>
-      <c r="I159" s="39"/>
-      <c r="J159" s="39"/>
-      <c r="K159" s="39"/>
-      <c r="L159" s="39"/>
+      <c r="B159" s="40"/>
+      <c r="C159" s="40"/>
+      <c r="D159" s="40"/>
+      <c r="E159" s="40"/>
+      <c r="F159" s="40"/>
+      <c r="G159" s="40"/>
+      <c r="H159" s="40"/>
+      <c r="I159" s="40"/>
+      <c r="J159" s="40"/>
+      <c r="K159" s="40"/>
+      <c r="L159" s="40"/>
     </row>
     <row r="160" spans="1:13">
       <c r="A160" s="9"/>
@@ -23319,14 +23298,14 @@
       <c r="K173" s="11"/>
     </row>
     <row r="174" spans="1:13">
-      <c r="A174" s="35" t="s">
+      <c r="A174" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="B174" s="35"/>
-      <c r="C174" s="35"/>
-      <c r="D174" s="35"/>
-      <c r="E174" s="35"/>
-      <c r="F174" s="35"/>
+      <c r="B174" s="36"/>
+      <c r="C174" s="36"/>
+      <c r="D174" s="36"/>
+      <c r="E174" s="36"/>
+      <c r="F174" s="36"/>
     </row>
     <row r="175" spans="1:13">
       <c r="B175" t="s">
@@ -23542,23 +23521,23 @@
       <c r="F187" s="13"/>
     </row>
     <row r="188" spans="1:13">
-      <c r="A188" s="35" t="s">
+      <c r="A188" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="B188" s="35"/>
-      <c r="C188" s="35"/>
-      <c r="D188" s="35"/>
-      <c r="E188" s="35"/>
+      <c r="B188" s="36"/>
+      <c r="C188" s="36"/>
+      <c r="D188" s="36"/>
+      <c r="E188" s="36"/>
       <c r="F188" s="32"/>
       <c r="G188" s="8"/>
-      <c r="H188" s="37" t="s">
+      <c r="H188" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="I188" s="37"/>
-      <c r="J188" s="37"/>
-      <c r="K188" s="37"/>
-      <c r="L188" s="37"/>
-      <c r="M188" s="37"/>
+      <c r="I188" s="39"/>
+      <c r="J188" s="39"/>
+      <c r="K188" s="39"/>
+      <c r="L188" s="39"/>
+      <c r="M188" s="39"/>
     </row>
     <row r="189" spans="1:13">
       <c r="B189" s="8" t="s">
@@ -23769,14 +23748,14 @@
       <c r="L194" s="1"/>
     </row>
     <row r="195" spans="1:14">
-      <c r="A195" s="34" t="s">
+      <c r="A195" s="35" t="s">
         <v>175</v>
       </c>
-      <c r="B195" s="34"/>
-      <c r="C195" s="34"/>
-      <c r="D195" s="34"/>
-      <c r="E195" s="34"/>
-      <c r="F195" s="34"/>
+      <c r="B195" s="35"/>
+      <c r="C195" s="35"/>
+      <c r="D195" s="35"/>
+      <c r="E195" s="35"/>
+      <c r="F195" s="35"/>
       <c r="H195" s="23"/>
       <c r="I195" s="23"/>
       <c r="J195" s="23"/>
@@ -23971,13 +23950,13 @@
       <c r="G202" s="11"/>
     </row>
     <row r="203" spans="1:14">
-      <c r="A203" s="34" t="s">
+      <c r="A203" s="35" t="s">
         <v>295</v>
       </c>
-      <c r="B203" s="34"/>
-      <c r="C203" s="34"/>
-      <c r="D203" s="34"/>
-      <c r="E203" s="34"/>
+      <c r="B203" s="35"/>
+      <c r="C203" s="35"/>
+      <c r="D203" s="35"/>
+      <c r="E203" s="35"/>
     </row>
     <row r="204" spans="1:14">
       <c r="B204" s="8" t="s">
@@ -24315,6 +24294,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A34:L34"/>
+    <mergeCell ref="A47:L47"/>
+    <mergeCell ref="A60:L60"/>
+    <mergeCell ref="A73:L73"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="E86:G86"/>
     <mergeCell ref="A188:E188"/>
     <mergeCell ref="H188:M188"/>
     <mergeCell ref="A195:F195"/>
@@ -24325,12 +24310,6 @@
     <mergeCell ref="A144:L144"/>
     <mergeCell ref="A159:L159"/>
     <mergeCell ref="A174:F174"/>
-    <mergeCell ref="A34:L34"/>
-    <mergeCell ref="A47:L47"/>
-    <mergeCell ref="A60:L60"/>
-    <mergeCell ref="A73:L73"/>
-    <mergeCell ref="A86:C86"/>
-    <mergeCell ref="E86:G86"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -25605,19 +25584,19 @@
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="36" t="s">
         <v>285</v>
       </c>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
     </row>
     <row r="12" spans="1:13">
       <c r="B12">
@@ -25659,7 +25638,7 @@
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="41" t="s">
         <v>283</v>
       </c>
       <c r="B13" s="1">
@@ -25701,7 +25680,7 @@
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="40"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="1">
         <v>0.1</v>
       </c>
@@ -25740,7 +25719,7 @@
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="40"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="1">
         <v>0.2</v>
       </c>
@@ -25779,7 +25758,7 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="40"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="1">
         <v>0.3</v>
       </c>
@@ -25818,7 +25797,7 @@
       </c>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="40"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="1">
         <v>0.4</v>
       </c>
@@ -25857,7 +25836,7 @@
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="40"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="1">
         <v>0.5</v>
       </c>
@@ -25896,7 +25875,7 @@
       </c>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="40"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="1">
         <v>0.6</v>
       </c>
@@ -25935,7 +25914,7 @@
       </c>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="40"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="1">
         <v>0.7</v>
       </c>
@@ -25974,7 +25953,7 @@
       </c>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="40"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="1">
         <v>0.8</v>
       </c>
@@ -26013,7 +25992,7 @@
       </c>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="40"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="1">
         <v>0.9</v>
       </c>
@@ -26052,7 +26031,7 @@
       </c>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="40"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="1">
         <v>1</v>
       </c>
@@ -26679,19 +26658,19 @@
       </c>
     </row>
     <row r="38" spans="1:13">
-      <c r="C38" s="35" t="s">
+      <c r="C38" s="36" t="s">
         <v>286</v>
       </c>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="35"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
-      <c r="K38" s="35"/>
-      <c r="L38" s="35"/>
-      <c r="M38" s="35"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="36"/>
+      <c r="L38" s="36"/>
+      <c r="M38" s="36"/>
     </row>
     <row r="39" spans="1:13">
       <c r="B39">
@@ -26733,7 +26712,7 @@
       </c>
     </row>
     <row r="40" spans="1:13">
-      <c r="A40" s="40" t="s">
+      <c r="A40" s="41" t="s">
         <v>284</v>
       </c>
       <c r="B40" s="1">
@@ -26775,7 +26754,7 @@
       </c>
     </row>
     <row r="41" spans="1:13">
-      <c r="A41" s="40"/>
+      <c r="A41" s="41"/>
       <c r="B41" s="1">
         <v>0.1</v>
       </c>
@@ -26814,7 +26793,7 @@
       </c>
     </row>
     <row r="42" spans="1:13">
-      <c r="A42" s="40"/>
+      <c r="A42" s="41"/>
       <c r="B42" s="1">
         <v>0.2</v>
       </c>
@@ -26853,7 +26832,7 @@
       </c>
     </row>
     <row r="43" spans="1:13">
-      <c r="A43" s="40"/>
+      <c r="A43" s="41"/>
       <c r="B43" s="1">
         <v>0.3</v>
       </c>
@@ -26892,7 +26871,7 @@
       </c>
     </row>
     <row r="44" spans="1:13">
-      <c r="A44" s="40"/>
+      <c r="A44" s="41"/>
       <c r="B44" s="1">
         <v>0.4</v>
       </c>
@@ -26931,7 +26910,7 @@
       </c>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="40"/>
+      <c r="A45" s="41"/>
       <c r="B45" s="1">
         <v>0.5</v>
       </c>
@@ -26970,7 +26949,7 @@
       </c>
     </row>
     <row r="46" spans="1:13">
-      <c r="A46" s="40"/>
+      <c r="A46" s="41"/>
       <c r="B46" s="1">
         <v>0.6</v>
       </c>
@@ -27009,7 +26988,7 @@
       </c>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" s="40"/>
+      <c r="A47" s="41"/>
       <c r="B47" s="1">
         <v>0.7</v>
       </c>
@@ -27048,7 +27027,7 @@
       </c>
     </row>
     <row r="48" spans="1:13">
-      <c r="A48" s="40"/>
+      <c r="A48" s="41"/>
       <c r="B48" s="1">
         <v>0.8</v>
       </c>
@@ -27087,7 +27066,7 @@
       </c>
     </row>
     <row r="49" spans="1:13">
-      <c r="A49" s="40"/>
+      <c r="A49" s="41"/>
       <c r="B49" s="1">
         <v>0.9</v>
       </c>
@@ -27126,7 +27105,7 @@
       </c>
     </row>
     <row r="50" spans="1:13">
-      <c r="A50" s="40"/>
+      <c r="A50" s="41"/>
       <c r="B50" s="1">
         <v>1</v>
       </c>
@@ -28832,10 +28811,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29087,9 +29066,11 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -29200,6 +29181,14 @@
       </c>
       <c r="B15" t="s">
         <v>322</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>20160928.199999999</v>
+      </c>
+      <c r="B16" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -29660,21 +29649,21 @@
     </row>
     <row r="4" spans="1:13" s="9" customFormat="1"/>
     <row r="5" spans="1:13">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="F5" s="34" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="F5" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="K5" s="34" t="s">
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="K5" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="27"/>
@@ -30069,16 +30058,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="35" t="str">
+      <c r="A1" s="36" t="str">
         <f>IF(Errors!B18="ERROR","WARNING: Inputs do not pass validation. Check that all percentages total to 100%","")</f>
         <v/>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
       <c r="H1" t="s">
         <v>312</v>
       </c>
@@ -30094,54 +30083,54 @@
       <c r="J2" s="29"/>
     </row>
     <row r="32" spans="5:18">
-      <c r="E32" s="36" t="s">
+      <c r="E32" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
       <c r="H32" s="11">
         <f>'RESULT-t''put'!B52</f>
         <v>0</v>
       </c>
-      <c r="K32" s="36" t="s">
+      <c r="K32" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="L32" s="36"/>
+      <c r="L32" s="37"/>
       <c r="M32" s="1">
         <f>'RESULT-t''put'!B73</f>
         <v>0.1809056799385467</v>
       </c>
-      <c r="P32" s="36" t="s">
+      <c r="P32" s="37" t="s">
         <v>223</v>
       </c>
-      <c r="Q32" s="36"/>
+      <c r="Q32" s="37"/>
       <c r="R32" s="1">
         <f>'RESULT-t''put'!B95</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="5:18">
-      <c r="E33" s="36" t="s">
+      <c r="E33" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
       <c r="H33" s="11">
         <f>'RESULT-t''put'!B53</f>
         <v>0</v>
       </c>
-      <c r="K33" s="36" t="s">
+      <c r="K33" s="37" t="s">
         <v>221</v>
       </c>
-      <c r="L33" s="36"/>
+      <c r="L33" s="37"/>
       <c r="M33" s="11">
         <f>'RESULT-t''put'!B74</f>
         <v>0.22086062069747245</v>
       </c>
-      <c r="P33" s="36" t="s">
+      <c r="P33" s="37" t="s">
         <v>224</v>
       </c>
-      <c r="Q33" s="36"/>
+      <c r="Q33" s="37"/>
       <c r="R33" s="1">
         <f>'RESULT-t''put'!B96</f>
         <v>0</v>
@@ -30207,16 +30196,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="35" t="str">
+      <c r="A1" s="36" t="str">
         <f>IF(Errors!B18="ERROR","WARNING: Inputs do not pass validation. Check that all percentages total to 100%","")</f>
         <v/>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
       <c r="H1" t="s">
         <v>312</v>
       </c>
@@ -30229,54 +30218,54 @@
       </c>
     </row>
     <row r="32" spans="5:18">
-      <c r="E32" s="36" t="s">
+      <c r="E32" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
       <c r="H32" s="11">
         <f>'RESULT-equal'!B28</f>
         <v>0</v>
       </c>
-      <c r="K32" s="36" t="s">
+      <c r="K32" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="L32" s="36"/>
+      <c r="L32" s="37"/>
       <c r="M32" s="1">
         <f>'RESULT-equal'!B49</f>
         <v>0.20003751834075728</v>
       </c>
-      <c r="P32" s="36" t="s">
+      <c r="P32" s="37" t="s">
         <v>223</v>
       </c>
-      <c r="Q32" s="36"/>
+      <c r="Q32" s="37"/>
       <c r="R32" s="1">
         <f>'RESULT-equal'!B71</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="5:18">
-      <c r="E33" s="36" t="s">
+      <c r="E33" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
       <c r="H33" s="11">
         <f>'RESULT-equal'!B29</f>
         <v>0</v>
       </c>
-      <c r="K33" s="36" t="s">
+      <c r="K33" s="37" t="s">
         <v>221</v>
       </c>
-      <c r="L33" s="36"/>
+      <c r="L33" s="37"/>
       <c r="M33" s="11">
         <f>'RESULT-equal'!B50</f>
         <v>0.25005862515683147</v>
       </c>
-      <c r="P33" s="36" t="s">
+      <c r="P33" s="37" t="s">
         <v>224</v>
       </c>
-      <c r="Q33" s="36"/>
+      <c r="Q33" s="37"/>
       <c r="R33" s="1">
         <f>'RESULT-equal'!B72</f>
         <v>0</v>

</xml_diff>